<commit_message>
Updated Python and LaTeX cheatsheet
</commit_message>
<xml_diff>
--- a/Basic LaTeX Cheatsheet.xlsx
+++ b/Basic LaTeX Cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A928C0FF-ABDF-459B-AC76-414CBFE69565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6825A9-9258-4BCD-AF04-ABCEC75724C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="16380" windowHeight="15585" firstSheet="1" activeTab="2" xr2:uid="{17074BF2-6FA4-45B9-A983-512215CEBAC8}"/>
+    <workbookView xWindow="28680" yWindow="5895" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{17074BF2-6FA4-45B9-A983-512215CEBAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="The Basics" sheetId="1" r:id="rId1"/>
@@ -483,47 +483,6 @@
     <t>Insert Title</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Inserts the title, date, and author in the document. Place inside </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>\begin{document}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>\end{document}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>Section Heading</t>
   </si>
   <si>
@@ -1884,6 +1843,9 @@
   </si>
   <si>
     <t>\text{ Text Mode Text }</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1966,7 +1928,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1990,29 +1952,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2113,6 +2057,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -2130,6 +2077,12 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2690,7 +2643,7 @@
     <tableColumn id="1" xr3:uid="{E6F8FB71-3344-446F-B4D9-A49B8CD38CF5}" name="Topic"/>
     <tableColumn id="2" xr3:uid="{171B8FB1-BDE0-4131-9BB5-17059BFF92A4}" name="Code"/>
     <tableColumn id="3" xr3:uid="{E78DBCE9-408C-4A0E-A929-266A7DFAA2D9}" name="Explained"/>
-    <tableColumn id="4" xr3:uid="{02649F9B-35A2-49A2-951A-D0EEE331E33C}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{02649F9B-35A2-49A2-951A-D0EEE331E33C}" name="Notes" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2703,49 +2656,49 @@
     <tableColumn id="1" xr3:uid="{43863EC7-2C89-42C6-A43C-D7CC77C96115}" name="Topic"/>
     <tableColumn id="2" xr3:uid="{28157D6F-83DD-41B9-BA1B-4F4C100A9DB2}" name="Code"/>
     <tableColumn id="3" xr3:uid="{47D62591-740C-41C9-BF03-B82CEC939C58}" name="Explained"/>
-    <tableColumn id="4" xr3:uid="{5B994B77-BA5A-4F3A-B6E0-43CD55CE5110}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{5B994B77-BA5A-4F3A-B6E0-43CD55CE5110}" name="Notes" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B5F10FF1-6A47-42C2-89E8-32CB60C645AE}" name="Table3" displayName="Table3" ref="A1:E14" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B5F10FF1-6A47-42C2-89E8-32CB60C645AE}" name="Table3" displayName="Table3" ref="A1:E14" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16">
   <autoFilter ref="A1:E14" xr:uid="{B5F10FF1-6A47-42C2-89E8-32CB60C645AE}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3EFC6834-D16F-4676-864B-2D10BC60B09B}" name="Topic" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{7C18B4A3-A643-44BC-A934-7A202E118C3B}" name="Code" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{BED9BF11-B198-4E77-B7CE-47C63B6504E0}" name="Explained" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{22289315-8071-4CAD-BBEE-7DAE745DD5A0}" name="Notes" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{8CC91188-7DE1-4E9A-A322-F97156F4B3B1}" name="Picture" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{3EFC6834-D16F-4676-864B-2D10BC60B09B}" name="Topic" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{7C18B4A3-A643-44BC-A934-7A202E118C3B}" name="Code" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{BED9BF11-B198-4E77-B7CE-47C63B6504E0}" name="Explained" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{22289315-8071-4CAD-BBEE-7DAE745DD5A0}" name="Notes" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{8CC91188-7DE1-4E9A-A322-F97156F4B3B1}" name="Picture" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{474CCE6D-AEBF-49A5-8E79-3401C3CED92A}" name="Table5" displayName="Table5" ref="A1:E7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{474CCE6D-AEBF-49A5-8E79-3401C3CED92A}" name="Table5" displayName="Table5" ref="A1:E7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
   <autoFilter ref="A1:E7" xr:uid="{474CCE6D-AEBF-49A5-8E79-3401C3CED92A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{306BF93D-00B5-48D1-B87A-5ADD7EF79B8A}" name="Topic"/>
     <tableColumn id="2" xr3:uid="{C297B8D9-F318-4C95-8002-12A890D1F202}" name="Code"/>
     <tableColumn id="3" xr3:uid="{80267582-C749-4E79-8C2B-828F00951437}" name="Explained"/>
     <tableColumn id="5" xr3:uid="{C4E9B21B-D410-4EF9-AB4F-A77606E77903}" name="Notes"/>
-    <tableColumn id="4" xr3:uid="{9D7A2302-2BB5-4162-8DAA-F198A98E2E66}" name="Picture" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{9D7A2302-2BB5-4162-8DAA-F198A98E2E66}" name="Picture" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{489CF9CA-F3A8-4C6C-9EA3-0E97294B6D77}" name="Table4" displayName="Table4" ref="A1:E14" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{489CF9CA-F3A8-4C6C-9EA3-0E97294B6D77}" name="Table4" displayName="Table4" ref="A1:E14" totalsRowShown="0" headerRowDxfId="4" dataDxfId="2" headerRowBorderDxfId="3" tableBorderDxfId="1">
   <autoFilter ref="A1:E14" xr:uid="{489CF9CA-F3A8-4C6C-9EA3-0E97294B6D77}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{45416AED-43E0-4E6F-B394-78078ACADCB8}" name="Topic"/>
     <tableColumn id="2" xr3:uid="{CEA129A3-9621-40BA-B1F3-D2CD52FF744A}" name="Code"/>
     <tableColumn id="3" xr3:uid="{6EEC5F35-0377-4D31-88D1-EC955283FC25}" name="Explained"/>
     <tableColumn id="5" xr3:uid="{BD2BB9BB-12DB-4BE8-818E-AC48AC02F0F9}" name="Notes"/>
-    <tableColumn id="4" xr3:uid="{C04A9FC6-8E44-43A1-B65F-756B683F751E}" name="Picture" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{C04A9FC6-8E44-43A1-B65F-756B683F751E}" name="Picture" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3082,6 +3035,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_GPT</we:customFunctionIds>
@@ -3118,6 +3074,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_AI_TABLE</we:customFunctionIds>
@@ -3138,7 +3097,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.7109375" defaultRowHeight="15"/>
@@ -3223,7 +3182,7 @@
         <v>62</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>63</v>
@@ -3237,7 +3196,7 @@
         <v>64</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>65</v>
@@ -3260,7 +3219,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45">
+    <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
         <v>69</v>
       </c>
@@ -3268,7 +3227,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>70</v>
+        <v>249</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>59</v>
@@ -3276,13 +3235,13 @@
     </row>
     <row r="10" spans="1:4" ht="30">
       <c r="A10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>59</v>
@@ -3290,13 +3249,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>59</v>
@@ -3304,41 +3263,41 @@
     </row>
     <row r="12" spans="1:4" ht="60">
       <c r="A12" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30">
       <c r="A13" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30">
       <c r="A14" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>59</v>
@@ -3346,13 +3305,13 @@
     </row>
     <row r="15" spans="1:4" ht="30">
       <c r="A15" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>59</v>
@@ -3360,13 +3319,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>59</v>
@@ -3374,13 +3333,13 @@
     </row>
     <row r="17" spans="1:4" ht="30">
       <c r="A17" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>59</v>
@@ -3388,13 +3347,13 @@
     </row>
     <row r="18" spans="1:4" ht="30">
       <c r="A18" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>59</v>
@@ -3402,13 +3361,13 @@
     </row>
     <row r="19" spans="1:4" ht="30">
       <c r="A19" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>59</v>
@@ -3416,13 +3375,13 @@
     </row>
     <row r="20" spans="1:4" ht="30">
       <c r="A20" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>59</v>
@@ -3430,13 +3389,13 @@
     </row>
     <row r="21" spans="1:4" ht="30">
       <c r="A21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>96</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>59</v>
@@ -3444,13 +3403,13 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>59</v>
@@ -3458,13 +3417,13 @@
     </row>
     <row r="23" spans="1:4" ht="30">
       <c r="A23" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>59</v>
@@ -3511,55 +3470,55 @@
     </row>
     <row r="2" spans="1:4" ht="45">
       <c r="A2" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45">
       <c r="A3" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
       <c r="A4" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>59</v>
@@ -3567,13 +3526,13 @@
     </row>
     <row r="6" spans="1:4" ht="30">
       <c r="A6" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>59</v>
@@ -3581,13 +3540,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>59</v>
@@ -3595,13 +3554,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>59</v>
@@ -3609,13 +3568,13 @@
     </row>
     <row r="9" spans="1:4" ht="60">
       <c r="A9" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>59</v>
@@ -3623,13 +3582,13 @@
     </row>
     <row r="10" spans="1:4" ht="45">
       <c r="A10" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>59</v>
@@ -3637,13 +3596,13 @@
     </row>
     <row r="11" spans="1:4" ht="60">
       <c r="A11" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>59</v>
@@ -3651,13 +3610,13 @@
     </row>
     <row r="12" spans="1:4" ht="38.25">
       <c r="A12" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>59</v>
@@ -3665,13 +3624,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>59</v>
@@ -3679,13 +3638,13 @@
     </row>
     <row r="14" spans="1:4" ht="42.75">
       <c r="A14" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>59</v>
@@ -3693,13 +3652,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>59</v>
@@ -3707,13 +3666,13 @@
     </row>
     <row r="16" spans="1:4" ht="30">
       <c r="A16" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>59</v>
@@ -3721,13 +3680,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>59</v>
@@ -3745,8 +3704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D92EB32-D779-43AF-A589-D08EAF458D75}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3777,28 +3736,28 @@
     </row>
     <row r="2" spans="1:5" ht="60">
       <c r="A2" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="30">
       <c r="A3" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>59</v>
@@ -3807,13 +3766,13 @@
     </row>
     <row r="4" spans="1:5" ht="30">
       <c r="A4" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>59</v>
@@ -3822,22 +3781,22 @@
     </row>
     <row r="5" spans="1:5" ht="60">
       <c r="A5" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="45">
+      <c r="A6" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="45">
-      <c r="A6" s="10" t="s">
-        <v>149</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>35</v>
@@ -3849,10 +3808,10 @@
     </row>
     <row r="7" spans="1:5" ht="120">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -3860,47 +3819,47 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" ht="120">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="195">
+      <c r="A9" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="195">
-      <c r="A9" s="10" t="s">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="195">
+      <c r="A10" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="195">
-      <c r="A10" s="10" t="s">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="135">
+      <c r="A11" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="135">
-      <c r="A11" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>36</v>
@@ -3911,41 +3870,41 @@
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="60">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="165">
+      <c r="A13" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="165">
-      <c r="A13" s="10" t="s">
+      <c r="D13" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -3995,13 +3954,13 @@
     </row>
     <row r="2" spans="1:5" ht="102">
       <c r="A2" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>173</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>174</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>59</v>
@@ -4012,13 +3971,13 @@
     </row>
     <row r="3" spans="1:5" ht="102">
       <c r="A3" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>176</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>59</v>
@@ -4029,33 +3988,33 @@
     </row>
     <row r="4" spans="1:5" ht="140.25">
       <c r="A4" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="E4" s="1" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="38.25">
+    <row r="5" spans="1:5" ht="60">
       <c r="A5" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>181</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>182</v>
       </c>
       <c r="E5" s="1" t="e" vm="4">
         <v>#VALUE!</v>
@@ -4063,13 +4022,13 @@
     </row>
     <row r="6" spans="1:5" ht="89.25">
       <c r="A6" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>183</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>184</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>59</v>
@@ -4080,13 +4039,13 @@
     </row>
     <row r="7" spans="1:5" ht="89.25">
       <c r="A7" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>185</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>186</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>59</v>
@@ -4108,7 +4067,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4139,170 +4098,170 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>200</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>40</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>203</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>204</v>
       </c>
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>229</v>
+        <v>196</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D11" s="7"/>
     </row>
     <row r="12" spans="1:5" ht="45">
       <c r="A12" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="48.75" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="60">
       <c r="A14" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -4318,8 +4277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D750F3F4-DB9C-496B-9927-CD4CF9E17BEE}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4347,68 +4306,68 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="30">
       <c r="A3" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:4" ht="60">
       <c r="A4" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>236</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45">
       <c r="A5" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>239</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="90">
       <c r="A6" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>242</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>